<commit_message>
Added more configs inside the Utils header file
</commit_message>
<xml_diff>
--- a/Docs/GPIO-Mapping.xlsx
+++ b/Docs/GPIO-Mapping.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
   <si>
     <t>Purpose</t>
   </si>
@@ -107,9 +107,6 @@
     <t>B6, B9, A4, C7, C10, C12, D4</t>
   </si>
   <si>
-    <t>A8-10, A13-15, C8,9,13-15, E0-4</t>
-  </si>
-  <si>
     <t>B12-15</t>
   </si>
   <si>
@@ -126,6 +123,18 @@
   </si>
   <si>
     <t>B4</t>
+  </si>
+  <si>
+    <t>A8-10, A13-15, C6,8,9,13-15, E0-3</t>
+  </si>
+  <si>
+    <t>Tempo</t>
+  </si>
+  <si>
+    <t>analogue</t>
+  </si>
+  <si>
+    <t>C4</t>
   </si>
 </sst>
 </file>
@@ -149,7 +158,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -213,6 +222,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -238,11 +253,11 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -557,10 +572,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X11"/>
+  <dimension ref="A1:X12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,7 +613,7 @@
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E2" s="6"/>
       <c r="I2">
@@ -671,7 +686,7 @@
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
-      <c r="M3" s="9"/>
+      <c r="M3" s="8"/>
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
@@ -703,9 +718,9 @@
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
-      <c r="M4" s="12"/>
-      <c r="O4" s="9"/>
-      <c r="R4" s="9"/>
+      <c r="M4" s="11"/>
+      <c r="O4" s="8"/>
+      <c r="R4" s="8"/>
       <c r="U4" s="5"/>
       <c r="V4" s="5"/>
       <c r="W4" s="5"/>
@@ -722,23 +737,23 @@
         <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="E5" s="4"/>
       <c r="H5" t="s">
         <v>21</v>
       </c>
       <c r="I5" s="3"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="9"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="12"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="8"/>
       <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
-      <c r="S5" s="9"/>
-      <c r="U5" s="9"/>
+      <c r="S5" s="8"/>
+      <c r="U5" s="8"/>
       <c r="V5" s="4"/>
       <c r="W5" s="4"/>
       <c r="X5" s="4"/>
@@ -754,9 +769,9 @@
         <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="10"/>
+        <v>29</v>
+      </c>
+      <c r="E6" s="9"/>
       <c r="H6" t="s">
         <v>22</v>
       </c>
@@ -764,7 +779,7 @@
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
-      <c r="M6" s="9"/>
+      <c r="M6" s="8"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -777,9 +792,9 @@
         <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="11"/>
+        <v>30</v>
+      </c>
+      <c r="E7" s="10"/>
       <c r="H7" t="s">
         <v>23</v>
       </c>
@@ -787,9 +802,9 @@
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
       <c r="P7" s="2"/>
       <c r="Q7" s="3"/>
       <c r="R7" s="3"/>
@@ -811,7 +826,7 @@
         <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E8" s="2"/>
     </row>
@@ -826,9 +841,9 @@
         <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="12"/>
+        <v>32</v>
+      </c>
+      <c r="E9" s="11"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -843,7 +858,7 @@
       <c r="D10" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="9"/>
+      <c r="E10" s="8"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -856,9 +871,24 @@
         <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
implemented code for reading GPIO pins.
Added some dead code to the other tasks.
Implemented some code for saving and changing songs.
</commit_message>
<xml_diff>
--- a/Docs/GPIO-Mapping.xlsx
+++ b/Docs/GPIO-Mapping.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
   <si>
     <t>Purpose</t>
   </si>
@@ -98,9 +98,6 @@
     <t>Port E</t>
   </si>
   <si>
-    <t>A0-3, A5-7, E8-15, C0</t>
-  </si>
-  <si>
     <t>B0-3</t>
   </si>
   <si>
@@ -135,6 +132,12 @@
   </si>
   <si>
     <t>C4</t>
+  </si>
+  <si>
+    <t>Not Used</t>
+  </si>
+  <si>
+    <t>A0-7, E8-15</t>
   </si>
 </sst>
 </file>
@@ -203,12 +206,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -228,6 +225,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -244,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -257,6 +260,7 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -575,7 +579,7 @@
   <dimension ref="A1:X12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,7 +617,7 @@
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E2" s="6"/>
       <c r="I2">
@@ -676,7 +680,7 @@
         <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E3" s="7"/>
       <c r="H3" t="s">
@@ -686,7 +690,7 @@
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
-      <c r="M3" s="8"/>
+      <c r="M3" s="3"/>
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
@@ -708,7 +712,7 @@
         <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="E4" s="3"/>
       <c r="H4" t="s">
@@ -718,9 +722,11 @@
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
-      <c r="M4" s="11"/>
-      <c r="O4" s="8"/>
-      <c r="R4" s="8"/>
+      <c r="M4" s="10"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="12"/>
       <c r="U4" s="5"/>
       <c r="V4" s="5"/>
       <c r="W4" s="5"/>
@@ -737,23 +743,23 @@
         <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E5" s="4"/>
       <c r="H5" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="11"/>
       <c r="O5" s="4"/>
-      <c r="P5" s="8"/>
+      <c r="P5" s="12"/>
       <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
-      <c r="S5" s="8"/>
-      <c r="U5" s="8"/>
+      <c r="S5" s="12"/>
+      <c r="U5" s="12"/>
       <c r="V5" s="4"/>
       <c r="W5" s="4"/>
       <c r="X5" s="4"/>
@@ -769,9 +775,9 @@
         <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="9"/>
+        <v>28</v>
+      </c>
+      <c r="E6" s="8"/>
       <c r="H6" t="s">
         <v>22</v>
       </c>
@@ -779,7 +785,7 @@
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
-      <c r="M6" s="8"/>
+      <c r="M6" s="12"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -792,9 +798,9 @@
         <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="10"/>
+        <v>29</v>
+      </c>
+      <c r="E7" s="9"/>
       <c r="H7" t="s">
         <v>23</v>
       </c>
@@ -802,9 +808,9 @@
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
       <c r="P7" s="2"/>
       <c r="Q7" s="3"/>
       <c r="R7" s="3"/>
@@ -826,7 +832,7 @@
         <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E8" s="2"/>
     </row>
@@ -841,24 +847,27 @@
         <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="11"/>
+        <v>31</v>
+      </c>
+      <c r="E9" s="10"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="13">
         <v>6</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="8"/>
+      <c r="D10" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -871,24 +880,24 @@
         <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" t="s">
         <v>35</v>
       </c>
-      <c r="D12" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" s="12"/>
+      <c r="E12" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Done with the skepeton code.
</commit_message>
<xml_diff>
--- a/Docs/GPIO-Mapping.xlsx
+++ b/Docs/GPIO-Mapping.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -113,18 +114,12 @@
     <t>E4-6</t>
   </si>
   <si>
-    <t>C1-3</t>
-  </si>
-  <si>
     <t>E7</t>
   </si>
   <si>
     <t>B4</t>
   </si>
   <si>
-    <t>A8-10, A13-15, C6,8,9,13-15, E0-3</t>
-  </si>
-  <si>
     <t>Tempo</t>
   </si>
   <si>
@@ -138,13 +133,19 @@
   </si>
   <si>
     <t>A0-7, E8-15</t>
+  </si>
+  <si>
+    <t>C0-2</t>
+  </si>
+  <si>
+    <t>A8-10, C3-11, E0-3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,8 +161,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -231,6 +239,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -247,7 +261,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -262,6 +276,8 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -579,7 +595,7 @@
   <dimension ref="A1:X12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -697,9 +713,11 @@
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
       <c r="S3" s="4"/>
-      <c r="V3" s="4"/>
-      <c r="W3" s="4"/>
-      <c r="X3" s="4"/>
+      <c r="T3" s="15"/>
+      <c r="U3" s="15"/>
+      <c r="V3" s="12"/>
+      <c r="W3" s="12"/>
+      <c r="X3" s="12"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -712,7 +730,7 @@
         <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E4" s="3"/>
       <c r="H4" t="s">
@@ -743,26 +761,28 @@
         <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E5" s="4"/>
       <c r="H5" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="12"/>
+      <c r="I5" s="14"/>
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="11"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
       <c r="O5" s="4"/>
-      <c r="P5" s="12"/>
+      <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
-      <c r="S5" s="12"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
       <c r="U5" s="12"/>
-      <c r="V5" s="4"/>
-      <c r="W5" s="4"/>
-      <c r="X5" s="4"/>
+      <c r="V5" s="12"/>
+      <c r="W5" s="12"/>
+      <c r="X5" s="12"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -798,7 +818,7 @@
         <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="E7" s="9"/>
       <c r="H7" t="s">
@@ -832,7 +852,7 @@
         <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E8" s="2"/>
     </row>
@@ -847,7 +867,7 @@
         <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E9" s="10"/>
     </row>
@@ -866,7 +886,7 @@
       </c>
       <c r="E10" s="13"/>
       <c r="F10" s="13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
@@ -886,16 +906,16 @@
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E12" s="11"/>
     </row>
@@ -903,4 +923,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated the GPIO mapping
</commit_message>
<xml_diff>
--- a/Docs/GPIO-Mapping.xlsx
+++ b/Docs/GPIO-Mapping.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -113,18 +114,12 @@
     <t>E4-6</t>
   </si>
   <si>
-    <t>C1-3</t>
-  </si>
-  <si>
     <t>E7</t>
   </si>
   <si>
     <t>B4</t>
   </si>
   <si>
-    <t>A8-10, A13-15, C6,8,9,13-15, E0-3</t>
-  </si>
-  <si>
     <t>Tempo</t>
   </si>
   <si>
@@ -138,13 +133,19 @@
   </si>
   <si>
     <t>A0-7, E8-15</t>
+  </si>
+  <si>
+    <t>C0-2</t>
+  </si>
+  <si>
+    <t>A8-10, C3-11, E0-3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,8 +161,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -231,6 +239,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -247,7 +261,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -262,6 +276,8 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -579,7 +595,7 @@
   <dimension ref="A1:X12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -697,9 +713,11 @@
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
       <c r="S3" s="4"/>
-      <c r="V3" s="4"/>
-      <c r="W3" s="4"/>
-      <c r="X3" s="4"/>
+      <c r="T3" s="15"/>
+      <c r="U3" s="15"/>
+      <c r="V3" s="12"/>
+      <c r="W3" s="12"/>
+      <c r="X3" s="12"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -712,7 +730,7 @@
         <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E4" s="3"/>
       <c r="H4" t="s">
@@ -743,26 +761,28 @@
         <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E5" s="4"/>
       <c r="H5" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="12"/>
+      <c r="I5" s="14"/>
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="11"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
       <c r="O5" s="4"/>
-      <c r="P5" s="12"/>
+      <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
-      <c r="S5" s="12"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
       <c r="U5" s="12"/>
-      <c r="V5" s="4"/>
-      <c r="W5" s="4"/>
-      <c r="X5" s="4"/>
+      <c r="V5" s="12"/>
+      <c r="W5" s="12"/>
+      <c r="X5" s="12"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -798,7 +818,7 @@
         <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="E7" s="9"/>
       <c r="H7" t="s">
@@ -832,7 +852,7 @@
         <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E8" s="2"/>
     </row>
@@ -847,7 +867,7 @@
         <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E9" s="10"/>
     </row>
@@ -866,7 +886,7 @@
       </c>
       <c r="E10" s="13"/>
       <c r="F10" s="13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
@@ -886,16 +906,16 @@
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E12" s="11"/>
     </row>
@@ -903,4 +923,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed an error when config GPIOs. Updated mappings
</commit_message>
<xml_diff>
--- a/Docs/GPIO-Mapping.xlsx
+++ b/Docs/GPIO-Mapping.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\OneDrive\School Work\EEE3074W Embedded Systems\ST080\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tino\OneDrive\School Work\EEE3074W Embedded Systems\ST080\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -126,9 +126,6 @@
     <t>analogue</t>
   </si>
   <si>
-    <t>C4</t>
-  </si>
-  <si>
     <t>Not Used</t>
   </si>
   <si>
@@ -139,6 +136,9 @@
   </si>
   <si>
     <t>A8-10, C3-11, E0-3</t>
+  </si>
+  <si>
+    <t>D4</t>
   </si>
 </sst>
 </file>
@@ -595,7 +595,7 @@
   <dimension ref="A1:X12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,7 +730,7 @@
         <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E4" s="3"/>
       <c r="H4" t="s">
@@ -761,7 +761,7 @@
         <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E5" s="4"/>
       <c r="H5" t="s">
@@ -805,7 +805,7 @@
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
-      <c r="M6" s="12"/>
+      <c r="M6" s="11"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -818,7 +818,7 @@
         <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E7" s="9"/>
       <c r="H7" t="s">
@@ -886,7 +886,7 @@
       </c>
       <c r="E10" s="13"/>
       <c r="F10" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
@@ -915,7 +915,7 @@
         <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E12" s="11"/>
     </row>

</xml_diff>

<commit_message>
Changed the gpio pins for channel rack
...and Added audio playback for compoer and playback
</commit_message>
<xml_diff>
--- a/Docs/GPIO-Mapping.xlsx
+++ b/Docs/GPIO-Mapping.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\OneDrive\School Work\EEE3074W Embedded Systems\ST080\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tino\OneDrive\School Work\EEE3074W Embedded Systems\ST080\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
   <si>
     <t>Purpose</t>
   </si>
@@ -132,13 +132,22 @@
     <t>Not Used</t>
   </si>
   <si>
-    <t>A0-7, E8-15</t>
-  </si>
-  <si>
     <t>C0-2</t>
   </si>
   <si>
     <t>A8-10, C3-11, E0-3</t>
+  </si>
+  <si>
+    <t>A0-3, D4, A5, D6-7, E8-15</t>
+  </si>
+  <si>
+    <t>Audio Out</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>A4</t>
   </si>
 </sst>
 </file>
@@ -169,7 +178,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -245,6 +254,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -261,7 +276,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -278,6 +293,7 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -592,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X12"/>
+  <dimension ref="A1:X13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -706,10 +722,10 @@
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
+      <c r="M3" s="16"/>
       <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
       <c r="S3" s="4"/>
@@ -730,7 +746,7 @@
         <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E4" s="3"/>
       <c r="H4" t="s">
@@ -761,7 +777,7 @@
         <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E5" s="4"/>
       <c r="H5" t="s">
@@ -805,7 +821,10 @@
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
-      <c r="M6" s="12"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -818,7 +837,7 @@
         <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E7" s="9"/>
       <c r="H7" t="s">
@@ -876,7 +895,7 @@
         <v>12</v>
       </c>
       <c r="B10" s="13">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>14</v>
@@ -918,6 +937,21 @@
         <v>33</v>
       </c>
       <c r="E12" s="11"/>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated the GPIO after chnages made by Othniel
</commit_message>
<xml_diff>
--- a/Docs/GPIO-Mapping.xlsx
+++ b/Docs/GPIO-Mapping.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\OneDrive\School Work\EEE3074W Embedded Systems\ST080\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\School\EEE3074W,2016\Project\ST080\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -144,7 +144,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -595,14 +595,14 @@
   <dimension ref="A1:X12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">

</xml_diff>